<commit_message>
updated FCR, updated plots 2024 Edition
</commit_message>
<xml_diff>
--- a/Data/FBOW_Sensitivity.xlsx
+++ b/Data/FBOW_Sensitivity.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\COWER_2023_gh\Annual_Reporting_Workflow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04D4FBD-762D-4A98-A3E8-90EA38143BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6513812A-3ACA-4B75-9750-FBE291C6A174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE68FA1B-042D-4330-8C4A-C1806BFF19D8}"/>
+    <workbookView xWindow="435" yWindow="255" windowWidth="11355" windowHeight="14580" xr2:uid="{EE68FA1B-042D-4330-8C4A-C1806BFF19D8}"/>
   </bookViews>
   <sheets>
-    <sheet name="FLOW_Sensitivity" sheetId="1" r:id="rId1"/>
+    <sheet name="FBOW_Sensitivity" sheetId="1" r:id="rId1"/>
     <sheet name="Fixed Charge Rates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -980,7 +980,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="44"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="44" applyAlignment="1">
@@ -1266,6 +1266,9 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="21" xfId="44" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="33" borderId="21" xfId="44" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="33" borderId="13" xfId="44" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1649,7 +1652,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1695,20 +1698,20 @@
       </c>
       <c r="B2">
         <f>($E$2*'Fixed Charge Rates'!$C$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>76.707832501292884</v>
+        <v>78.661019548054909</v>
       </c>
       <c r="C2">
         <f>($F$2*'Fixed Charge Rates'!$C$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>113.10402831267888</v>
+        <v>116.62686558569571</v>
       </c>
       <c r="D2">
         <f>($G$2*'Fixed Charge Rates'!$C$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>137.09375119931298</v>
+        <v>141.65118764175773</v>
       </c>
       <c r="E2">
         <v>3000</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="121">
         <v>5410.9061579999998</v>
       </c>
       <c r="G2">
@@ -1724,21 +1727,21 @@
       </c>
       <c r="B3">
         <f>($F$2*'Fixed Charge Rates'!$C$19+$E$3)/($F$4/100*8760/1000)</f>
-        <v>97.394831573789986</v>
+        <v>100.91766884680681</v>
       </c>
       <c r="C3">
         <f>($F$2*'Fixed Charge Rates'!$C$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>113.10402831267888</v>
+        <v>116.62686558569571</v>
       </c>
       <c r="D3">
         <f>($F$2*'Fixed Charge Rates'!$C$19+$G$3)/($F$4/100*8760/1000)</f>
-        <v>128.81322505156777</v>
+        <v>132.33606232458462</v>
       </c>
       <c r="E3">
         <f>F3*0.5</f>
         <v>67.471000000000004</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="121">
         <v>134.94200000000001</v>
       </c>
       <c r="G3">
@@ -1755,20 +1758,20 @@
       </c>
       <c r="B4">
         <f>($F$2*'Fixed Charge Rates'!$C$19+$F$3)/($E$4/100*8760/1000)</f>
-        <v>100.82644284963776</v>
+        <v>103.96687167675663</v>
       </c>
       <c r="C4">
         <f>($F$2*'Fixed Charge Rates'!$C$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>113.10402831267888</v>
+        <v>116.62686558569571</v>
       </c>
       <c r="D4">
         <f>($F$2*'Fixed Charge Rates'!$C$19+$F$3)/($G$4/100*8760/1000)</f>
-        <v>158.44155304943075</v>
+        <v>163.37651263490326</v>
       </c>
       <c r="E4">
         <v>55</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="120">
         <v>49.029680370000001</v>
       </c>
       <c r="G4">
@@ -1784,26 +1787,27 @@
       </c>
       <c r="B5">
         <f>($F$2*'Fixed Charge Rates'!$D$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>99.526325635273423</v>
+        <v>101.90965618418579</v>
       </c>
       <c r="C5">
         <f>($F$2*'Fixed Charge Rates'!$C$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>113.10402831267888</v>
+        <v>116.62686558569571</v>
       </c>
       <c r="D5">
         <f>($F$2*'Fixed Charge Rates'!$E$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>128.02470719254993</v>
+        <v>132.83682694854977</v>
       </c>
       <c r="E5">
         <f>F5*0.75</f>
-        <v>4.6725000000000003</v>
-      </c>
-      <c r="F5">
-        <v>6.23</v>
+        <v>4.9579004999999992</v>
+      </c>
+      <c r="F5" s="119">
+        <f>'Fixed Charge Rates'!C10*100</f>
+        <v>6.6105339999999995</v>
       </c>
       <c r="G5">
         <f>F5*1.25</f>
-        <v>7.7875000000000005</v>
+        <v>8.2631674999999998</v>
       </c>
       <c r="H5" t="s">
         <v>52</v>
@@ -1815,15 +1819,15 @@
       </c>
       <c r="B6">
         <f>($F$2*'Fixed Charge Rates'!$G$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>99.031540512311068</v>
+        <v>102.7589926579837</v>
       </c>
       <c r="C6">
         <f>($F$2*'Fixed Charge Rates'!$C$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>113.10402831267888</v>
+        <v>116.62686558569571</v>
       </c>
       <c r="D6">
         <f>($F$2*'Fixed Charge Rates'!$F$19+$F$3)/($F$4/100*8760/1000)</f>
-        <v>147.70764136846159</v>
+        <v>151.09802348579476</v>
       </c>
       <c r="E6">
         <v>35</v>
@@ -1848,7 +1852,7 @@
   <dimension ref="A1:AO130"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.7109375" defaultRowHeight="15"/>
@@ -2160,19 +2164,19 @@
         <v>13</v>
       </c>
       <c r="C7" s="22">
-        <v>0.6</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="D7" s="22">
-        <v>0.6</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="E7" s="22">
-        <v>0.6</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="F7" s="22">
-        <v>0.6</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="G7" s="22">
-        <v>0.6</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="H7" s="43"/>
       <c r="I7" s="15"/>
@@ -2208,19 +2212,19 @@
         <v>13</v>
       </c>
       <c r="C8" s="23">
-        <v>5.8999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D8" s="23">
-        <v>5.8999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E8" s="23">
-        <v>5.8999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F8" s="23">
-        <v>5.8999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G8" s="23">
-        <v>5.8999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="113"/>
@@ -2255,19 +2259,19 @@
         <v>13</v>
       </c>
       <c r="C9" s="23">
-        <v>0.09</v>
+        <v>0.105</v>
       </c>
       <c r="D9" s="23">
-        <v>0.09</v>
+        <v>0.105</v>
       </c>
       <c r="E9" s="23">
-        <v>0.09</v>
+        <v>0.105</v>
       </c>
       <c r="F9" s="23">
-        <v>0.09</v>
+        <v>0.105</v>
       </c>
       <c r="G9" s="23">
-        <v>0.09</v>
+        <v>0.105</v>
       </c>
       <c r="H9" s="44"/>
       <c r="I9" s="15"/>
@@ -2304,23 +2308,23 @@
       </c>
       <c r="C10" s="25">
         <f>C7*(C8*(1-C3))+(1-C7)*C9</f>
-        <v>6.2302199999999988E-2</v>
+        <v>6.6105339999999999E-2</v>
       </c>
       <c r="D10" s="25">
-        <f>FLOW_Sensitivity!E5/100</f>
-        <v>4.6725000000000003E-2</v>
+        <f>FBOW_Sensitivity!E5/100</f>
+        <v>4.9579004999999989E-2</v>
       </c>
       <c r="E10" s="25">
-        <f>FLOW_Sensitivity!G5/100</f>
-        <v>7.7875E-2</v>
+        <f>FBOW_Sensitivity!G5/100</f>
+        <v>8.2631675000000002E-2</v>
       </c>
       <c r="F10" s="25">
         <f>F7*(F8*(1-F3))+(1-F7)*F9</f>
-        <v>6.2302199999999988E-2</v>
+        <v>6.6105339999999999E-2</v>
       </c>
       <c r="G10" s="25">
         <f>G7*(G8*(1-G3))+(1-G7)*G9</f>
-        <v>6.2302199999999988E-2</v>
+        <v>6.6105339999999999E-2</v>
       </c>
       <c r="H10" s="45"/>
       <c r="I10" s="15" t="s">
@@ -2376,23 +2380,23 @@
       </c>
       <c r="C11" s="25">
         <f>(1+C10)/(1+C6)-1</f>
-        <v>3.6392390243902506E-2</v>
+        <v>4.0102770731707427E-2</v>
       </c>
       <c r="D11" s="25">
         <f>(1+D10)/(1+D6)-1</f>
-        <v>2.119512195121942E-2</v>
+        <v>2.397951707317092E-2</v>
       </c>
       <c r="E11" s="25">
         <f>(1+E10)/(1+E6)-1</f>
-        <v>5.1585365853658471E-2</v>
+        <v>5.6226024390243934E-2</v>
       </c>
       <c r="F11" s="25">
         <f>(1+F10)/(1+F6)-1</f>
-        <v>3.6392390243902506E-2</v>
+        <v>4.0102770731707427E-2</v>
       </c>
       <c r="G11" s="25">
         <f>(1+G10)/(1+G6)-1</f>
-        <v>3.6392390243902506E-2</v>
+        <v>4.0102770731707427E-2</v>
       </c>
       <c r="H11" s="47"/>
       <c r="I11" s="15" t="s">
@@ -2458,23 +2462,23 @@
       </c>
       <c r="C12" s="27">
         <f>(C10*(1+C10)^C2)/((1+C10)^C2-1)</f>
-        <v>7.9946135059757464E-2</v>
+        <v>8.2821673860960399E-2</v>
       </c>
       <c r="D12" s="27">
         <f>(D10*(1+D10)^D2)/((1+D10)^D2-1)</f>
-        <v>6.8641547512808654E-2</v>
+        <v>7.0653370938200108E-2</v>
       </c>
       <c r="E12" s="27">
         <f>(E10*(1+E10)^E2)/((1+E10)^E2-1)</f>
-        <v>9.1984233314842317E-2</v>
+        <v>9.5793559635582781E-2</v>
       </c>
       <c r="F12" s="27">
         <f>(F10*(1+F10)^F2)/((1+F10)^F2-1)</f>
-        <v>0.10451716079057544</v>
+        <v>0.10710923873896827</v>
       </c>
       <c r="G12" s="27">
         <f>(G10*(1+G10)^G2)/((1+G10)^G2-1)</f>
-        <v>7.0845584590653723E-2</v>
+        <v>7.3977532134242796E-2</v>
       </c>
       <c r="H12" s="48"/>
       <c r="I12" s="15" t="s">
@@ -2560,23 +2564,23 @@
       </c>
       <c r="C13" s="10">
         <f>(C11*(1+C11)^C2)/((1+C11)^C2-1)</f>
-        <v>6.1594465433041604E-2</v>
+        <v>6.4081515203388131E-2</v>
       </c>
       <c r="D13" s="10">
         <f>(D11*(1+D11)^D2)/((1+D11)^D2-1)</f>
-        <v>5.1941887684484336E-2</v>
+        <v>5.3644402735243762E-2</v>
       </c>
       <c r="E13" s="10">
         <f>(E11*(1+E11)^E2)/((1+E11)^E2-1)</f>
-        <v>7.2084040280713149E-2</v>
+        <v>7.5443731118044963E-2</v>
       </c>
       <c r="F13" s="10">
         <f>(F11*(1+F11)^F2)/((1+F11)^F2-1)</f>
-        <v>8.7687070975382267E-2</v>
+        <v>9.0005745205492857E-2</v>
       </c>
       <c r="G13" s="10">
         <f>(G11*(1+G11)^G2)/((1+G11)^G2-1)</f>
-        <v>5.0983207221869435E-2</v>
+        <v>5.3652102635934604E-2</v>
       </c>
       <c r="H13" s="49"/>
       <c r="I13" s="15" t="s">
@@ -2778,23 +2782,23 @@
       </c>
       <c r="C16" s="30">
         <f>NPV(C$10,$L6:$Q6)</f>
-        <v>0.84769390092534425</v>
+        <v>0.83965254641178855</v>
       </c>
       <c r="D16" s="30">
         <f>NPV(D$10,$L6:$Q6)</f>
-        <v>0.88200461379327422</v>
+        <v>0.87554780856298875</v>
       </c>
       <c r="E16" s="30">
         <f>NPV(E$10,$L6:$Q6)</f>
-        <v>0.81555401594780896</v>
+        <v>0.80613988877574361</v>
       </c>
       <c r="F16" s="30">
         <f>NPV(F$10,$L6:$Q6)</f>
-        <v>0.84769390092534425</v>
+        <v>0.83965254641178855</v>
       </c>
       <c r="G16" s="30">
         <f>NPV(G$10,$L6:$Q6)</f>
-        <v>0.84769390092534425</v>
+        <v>0.83965254641178855</v>
       </c>
       <c r="H16" s="54"/>
       <c r="I16" s="54"/>
@@ -2834,23 +2838,23 @@
       </c>
       <c r="C17" s="31">
         <f>(1-C3*C16)/(1-C3)</f>
-        <v>1.0526819212142484</v>
+        <v>1.0554633856960569</v>
       </c>
       <c r="D17" s="31">
         <f>(1-D3*D16)/(1-D3)</f>
-        <v>1.0408140164941164</v>
+        <v>1.0430473932695987</v>
       </c>
       <c r="E17" s="31">
         <f>(1-E3*E16)/(1-E3)</f>
-        <v>1.0637989473774065</v>
+        <v>1.0670552470856445</v>
       </c>
       <c r="F17" s="31">
         <f>(1-F3*F16)/(1-F3)</f>
-        <v>1.0526819212142484</v>
+        <v>1.0554633856960569</v>
       </c>
       <c r="G17" s="31">
         <f>(1-G3*G16)/(1-G3)</f>
-        <v>1.0526819212142484</v>
+        <v>1.0554633856960569</v>
       </c>
       <c r="H17" s="45"/>
       <c r="I17" s="45"/>
@@ -2890,23 +2894,23 @@
       </c>
       <c r="C18" s="33">
         <f>C12*C17</f>
-        <v>8.4157851048359267E-2</v>
+        <v>8.7415244302303879E-2</v>
       </c>
       <c r="D18" s="33">
         <f>D12*D17</f>
-        <v>7.1443084765178105E-2</v>
+        <v>7.369481438279965E-2</v>
       </c>
       <c r="E18" s="33">
         <f>E12*E17</f>
-        <v>9.7852730575647029E-2</v>
+        <v>0.1022170204461602</v>
       </c>
       <c r="F18" s="33">
         <f>F12*F17</f>
-        <v>0.11002332562088146</v>
+        <v>0.11304987975875871</v>
       </c>
       <c r="G18" s="33">
         <f>G12*G17</f>
-        <v>7.4577866096435921E-2</v>
+        <v>7.8080576531846746E-2</v>
       </c>
       <c r="H18" s="54"/>
       <c r="I18" s="54"/>
@@ -2946,23 +2950,23 @@
       </c>
       <c r="C19" s="33">
         <f>C13*C17</f>
-        <v>6.4839380208218847E-2</v>
+        <v>6.7635692997101385E-2</v>
       </c>
       <c r="D19" s="33">
         <f>D13*D17</f>
-        <v>5.406184474517442E-2</v>
+        <v>5.5953654436500536E-2</v>
       </c>
       <c r="E19" s="33">
         <f>E13*E17</f>
-        <v>7.6682926173333221E-2</v>
+        <v>8.0502629149228386E-2</v>
       </c>
       <c r="F19" s="33">
         <f>F13*F17</f>
-        <v>9.2306594340015563E-2</v>
+        <v>9.4997768566686139E-2</v>
       </c>
       <c r="G19" s="33">
         <f>G13*G17</f>
-        <v>5.3669100527981663E-2</v>
+        <v>5.662782989783588E-2</v>
       </c>
       <c r="H19" s="45"/>
       <c r="I19" s="45"/>
@@ -6533,4 +6537,10 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{95965d95-ecc0-4720-b759-1f33c42ed7da}" enabled="1" method="Standard" siteId="{a0f29d7e-28cd-4f54-8442-7885aee7c080}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>